<commit_message>
realice la modificacion de la plantila excel para corregir el formato, se modifico el codigo de control_reporte para ajustar a la nueva plantilla
</commit_message>
<xml_diff>
--- a/Archivos/reporte.xlsx
+++ b/Archivos/reporte.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\coso\pp_webpage\Archivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\actualizacion\pp_webpage\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5CA86E-6A2E-41D8-8DEF-A7C6B2E0C9F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CA8599-064C-4528-8717-4F4ADCFFF565}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -670,11 +670,29 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -685,26 +703,80 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -717,90 +789,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -872,7 +860,7 @@
             <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
           </a:ext>
           <a:ext uri="{FAA26D3D-D897-4be2-8F04-BA451C77F1D7}">
-            <ma14:placeholderFlag xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns="" xmlns:arto="http://schemas.microsoft.com/office/word/2006/arto" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" xmlns:cx8="http://schemas.microsoft.com/office/drawing/2016/5/14/chartex" xmlns:cx7="http://schemas.microsoft.com/office/drawing/2016/5/13/chartex" xmlns:cx6="http://schemas.microsoft.com/office/drawing/2016/5/12/chartex" xmlns:cx5="http://schemas.microsoft.com/office/drawing/2016/5/11/chartex" xmlns:cx4="http://schemas.microsoft.com/office/drawing/2016/5/10/chartex" xmlns:cx3="http://schemas.microsoft.com/office/drawing/2016/5/9/chartex" xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas"/>
+            <ma14:placeholderFlag xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" xmlns:cx3="http://schemas.microsoft.com/office/drawing/2016/5/9/chartex" xmlns:cx4="http://schemas.microsoft.com/office/drawing/2016/5/10/chartex" xmlns:cx5="http://schemas.microsoft.com/office/drawing/2016/5/11/chartex" xmlns:cx6="http://schemas.microsoft.com/office/drawing/2016/5/12/chartex" xmlns:cx7="http://schemas.microsoft.com/office/drawing/2016/5/13/chartex" xmlns:cx8="http://schemas.microsoft.com/office/drawing/2016/5/14/chartex" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:arto="http://schemas.microsoft.com/office/word/2006/arto" xmlns="" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -1203,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:B57"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60:J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1241,25 +1229,25 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="20.25">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
     </row>
     <row r="4" spans="1:13" ht="15.75">
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:13" ht="15">
       <c r="B5" s="2" t="s">
@@ -1278,23 +1266,23 @@
       <c r="H6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="39"/>
-      <c r="J6" s="40"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="64"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1"/>
     <row r="8" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="31"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="37"/>
     </row>
     <row r="9" spans="1:13" ht="15">
       <c r="A9" s="2" t="s">
@@ -1304,13 +1292,13 @@
       <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
       <c r="H9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
     </row>
     <row r="11" spans="1:13" ht="66.75" customHeight="1">
       <c r="A11" s="2" t="s">
@@ -1321,13 +1309,13 @@
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
       <c r="H11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1">
       <c r="C12" s="4"/>
@@ -1338,18 +1326,18 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="31"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="37"/>
       <c r="M13" s="26" t="s">
         <v>45</v>
       </c>
@@ -1358,57 +1346,57 @@
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
     </row>
     <row r="16" spans="1:13" ht="15">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
     </row>
     <row r="18" spans="1:10" ht="39" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
     </row>
     <row r="20" spans="1:10" ht="32.25" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="66"/>
     </row>
     <row r="22" spans="1:10" ht="15">
       <c r="A22" s="2" t="s">
@@ -1418,12 +1406,12 @@
       <c r="D22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
     </row>
     <row r="23" spans="1:10">
       <c r="B23" s="24"/>
@@ -1438,26 +1426,26 @@
       <c r="D24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
     </row>
     <row r="26" spans="1:10" ht="15">
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="40"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="64"/>
       <c r="F26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="39">
+      <c r="I26" s="63">
         <v>43830</v>
       </c>
-      <c r="J26" s="40"/>
+      <c r="J26" s="64"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1">
       <c r="A27" s="2"/>
@@ -1468,142 +1456,142 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="31"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A29" s="65" t="s">
+      <c r="A29" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="65" t="s">
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="J29" s="67"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A30" s="35"/>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="70"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="28"/>
     </row>
     <row r="31" spans="1:10" ht="15" thickBot="1">
-      <c r="A31" s="35"/>
-      <c r="B31" s="68"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="70"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="28"/>
     </row>
     <row r="32" spans="1:10" ht="15" thickBot="1">
-      <c r="A32" s="35"/>
-      <c r="B32" s="68"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="70"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="28"/>
     </row>
     <row r="33" spans="1:10" ht="15" thickBot="1">
-      <c r="A33" s="35"/>
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="70"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="28"/>
     </row>
     <row r="34" spans="1:10" ht="15" thickBot="1">
-      <c r="A34" s="35"/>
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="70"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="28"/>
     </row>
     <row r="35" spans="1:10" ht="15" thickBot="1">
-      <c r="A35" s="35"/>
-      <c r="B35" s="68"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="68"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="70"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="28"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="35"/>
-      <c r="B36" s="68"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="68"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="69"/>
-      <c r="J36" s="70"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="28"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1">
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="31"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="37"/>
     </row>
     <row r="39" spans="1:10" ht="45.75" thickBot="1">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="45"/>
+      <c r="B39" s="49"/>
       <c r="C39" s="17" t="s">
         <v>7</v>
       </c>
@@ -1630,8 +1618,8 @@
       </c>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="35"/>
-      <c r="B40" s="36"/>
+      <c r="A40" s="32"/>
+      <c r="B40" s="34"/>
       <c r="C40" s="18"/>
       <c r="D40" s="19"/>
       <c r="E40" s="19"/>
@@ -1642,8 +1630,8 @@
       <c r="J40" s="20"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="37"/>
-      <c r="B41" s="38"/>
+      <c r="A41" s="44"/>
+      <c r="B41" s="45"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -1654,8 +1642,8 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="37"/>
-      <c r="B42" s="38"/>
+      <c r="A42" s="44"/>
+      <c r="B42" s="45"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -1666,8 +1654,8 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="37"/>
-      <c r="B43" s="38"/>
+      <c r="A43" s="44"/>
+      <c r="B43" s="45"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -1678,8 +1666,8 @@
       <c r="J43" s="6"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="37"/>
-      <c r="B44" s="38"/>
+      <c r="A44" s="44"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
@@ -1690,8 +1678,8 @@
       <c r="J44" s="6"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="37"/>
-      <c r="B45" s="38"/>
+      <c r="A45" s="44"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -1702,8 +1690,8 @@
       <c r="J45" s="6"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="37"/>
-      <c r="B46" s="38"/>
+      <c r="A46" s="44"/>
+      <c r="B46" s="45"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -1714,8 +1702,8 @@
       <c r="J46" s="6"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="37"/>
-      <c r="B47" s="38"/>
+      <c r="A47" s="44"/>
+      <c r="B47" s="45"/>
       <c r="C47" s="5"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
@@ -1726,8 +1714,8 @@
       <c r="J47" s="6"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="37"/>
-      <c r="B48" s="38"/>
+      <c r="A48" s="44"/>
+      <c r="B48" s="45"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -1738,8 +1726,8 @@
       <c r="J48" s="6"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="37"/>
-      <c r="B49" s="38"/>
+      <c r="A49" s="44"/>
+      <c r="B49" s="45"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -1750,8 +1738,8 @@
       <c r="J49" s="6"/>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="37"/>
-      <c r="B50" s="38"/>
+      <c r="A50" s="44"/>
+      <c r="B50" s="45"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -1762,8 +1750,8 @@
       <c r="J50" s="6"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="37"/>
-      <c r="B51" s="38"/>
+      <c r="A51" s="44"/>
+      <c r="B51" s="45"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -1774,8 +1762,8 @@
       <c r="J51" s="6"/>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="37"/>
-      <c r="B52" s="38"/>
+      <c r="A52" s="44"/>
+      <c r="B52" s="45"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
@@ -1786,8 +1774,8 @@
       <c r="J52" s="6"/>
     </row>
     <row r="53" spans="1:10" ht="15" thickBot="1">
-      <c r="A53" s="48"/>
-      <c r="B53" s="49"/>
+      <c r="A53" s="39"/>
+      <c r="B53" s="40"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
@@ -1810,38 +1798,38 @@
       <c r="J54" s="10"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="54"/>
-      <c r="E55" s="54"/>
-      <c r="F55" s="54"/>
-      <c r="G55" s="54"/>
-      <c r="H55" s="54"/>
-      <c r="I55" s="54"/>
-      <c r="J55" s="55"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="52"/>
+      <c r="G55" s="52"/>
+      <c r="H55" s="52"/>
+      <c r="I55" s="52"/>
+      <c r="J55" s="53"/>
     </row>
     <row r="56" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A56" s="44" t="s">
+      <c r="A56" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="45"/>
+      <c r="B56" s="49"/>
       <c r="C56" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D56" s="56" t="s">
+      <c r="D56" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="E56" s="57"/>
-      <c r="F56" s="57"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="59" t="s">
+      <c r="E56" s="55"/>
+      <c r="F56" s="55"/>
+      <c r="G56" s="56"/>
+      <c r="H56" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="I56" s="60"/>
-      <c r="J56" s="61"/>
+      <c r="I56" s="58"/>
+      <c r="J56" s="59"/>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="50" t="s">
@@ -1849,181 +1837,181 @@
       </c>
       <c r="B57" s="51"/>
       <c r="C57" s="11"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
-      <c r="J57" s="43"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="38"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="52"/>
-      <c r="B58" s="53"/>
+      <c r="A58" s="46"/>
+      <c r="B58" s="47"/>
       <c r="C58" s="12"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
-      <c r="H58" s="43"/>
-      <c r="I58" s="43"/>
-      <c r="J58" s="43"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="38"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+      <c r="J58" s="38"/>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="52"/>
-      <c r="B59" s="53"/>
+      <c r="A59" s="46"/>
+      <c r="B59" s="47"/>
       <c r="C59" s="12"/>
-      <c r="D59" s="43"/>
-      <c r="E59" s="43"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="43"/>
-      <c r="H59" s="43"/>
-      <c r="I59" s="43"/>
-      <c r="J59" s="43"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="38"/>
+      <c r="H59" s="38"/>
+      <c r="I59" s="38"/>
+      <c r="J59" s="38"/>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="37"/>
-      <c r="B60" s="38"/>
+      <c r="A60" s="44"/>
+      <c r="B60" s="45"/>
       <c r="C60" s="12"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
-      <c r="H60" s="33"/>
-      <c r="I60" s="33"/>
-      <c r="J60" s="34"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="38"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="37"/>
-      <c r="B61" s="38"/>
+      <c r="A61" s="44"/>
+      <c r="B61" s="45"/>
       <c r="C61" s="12"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="33"/>
-      <c r="H61" s="33"/>
-      <c r="I61" s="33"/>
-      <c r="J61" s="34"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="38"/>
+      <c r="I61" s="38"/>
+      <c r="J61" s="38"/>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="37"/>
-      <c r="B62" s="38"/>
+      <c r="A62" s="44"/>
+      <c r="B62" s="45"/>
       <c r="C62" s="12"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="33"/>
-      <c r="J62" s="34"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="38"/>
+      <c r="I62" s="38"/>
+      <c r="J62" s="38"/>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="37"/>
-      <c r="B63" s="38"/>
+      <c r="A63" s="44"/>
+      <c r="B63" s="45"/>
       <c r="C63" s="12"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
-      <c r="H63" s="33"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="34"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="38"/>
+      <c r="I63" s="38"/>
+      <c r="J63" s="38"/>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="37"/>
-      <c r="B64" s="38"/>
+      <c r="A64" s="44"/>
+      <c r="B64" s="45"/>
       <c r="C64" s="12"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="33"/>
-      <c r="F64" s="33"/>
-      <c r="G64" s="33"/>
-      <c r="H64" s="33"/>
-      <c r="I64" s="33"/>
-      <c r="J64" s="34"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="37"/>
-      <c r="B65" s="38"/>
+      <c r="A65" s="44"/>
+      <c r="B65" s="45"/>
       <c r="C65" s="12"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="33"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="33"/>
-      <c r="H65" s="33"/>
-      <c r="I65" s="33"/>
-      <c r="J65" s="34"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="38"/>
+      <c r="H65" s="38"/>
+      <c r="I65" s="38"/>
+      <c r="J65" s="38"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="37"/>
-      <c r="B66" s="38"/>
+      <c r="A66" s="44"/>
+      <c r="B66" s="45"/>
       <c r="C66" s="12"/>
-      <c r="D66" s="33"/>
-      <c r="E66" s="33"/>
-      <c r="F66" s="33"/>
-      <c r="G66" s="33"/>
-      <c r="H66" s="33"/>
-      <c r="I66" s="33"/>
-      <c r="J66" s="34"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="38"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
+      <c r="J66" s="38"/>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="37"/>
-      <c r="B67" s="38"/>
+      <c r="A67" s="44"/>
+      <c r="B67" s="45"/>
       <c r="C67" s="12"/>
-      <c r="D67" s="33"/>
-      <c r="E67" s="33"/>
-      <c r="F67" s="33"/>
-      <c r="G67" s="33"/>
-      <c r="H67" s="33"/>
-      <c r="I67" s="33"/>
-      <c r="J67" s="34"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="38"/>
+      <c r="G67" s="38"/>
+      <c r="H67" s="38"/>
+      <c r="I67" s="38"/>
+      <c r="J67" s="38"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="37"/>
-      <c r="B68" s="38"/>
+      <c r="A68" s="44"/>
+      <c r="B68" s="45"/>
       <c r="C68" s="12"/>
-      <c r="D68" s="33"/>
-      <c r="E68" s="33"/>
-      <c r="F68" s="33"/>
-      <c r="G68" s="33"/>
-      <c r="H68" s="33"/>
-      <c r="I68" s="33"/>
-      <c r="J68" s="34"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="38"/>
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
+      <c r="J68" s="38"/>
     </row>
     <row r="69" spans="1:10">
-      <c r="A69" s="37"/>
-      <c r="B69" s="38"/>
+      <c r="A69" s="44"/>
+      <c r="B69" s="45"/>
       <c r="C69" s="12"/>
-      <c r="D69" s="33"/>
-      <c r="E69" s="33"/>
-      <c r="F69" s="33"/>
-      <c r="G69" s="33"/>
-      <c r="H69" s="33"/>
-      <c r="I69" s="33"/>
-      <c r="J69" s="34"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+      <c r="I69" s="38"/>
+      <c r="J69" s="38"/>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="37"/>
-      <c r="B70" s="38"/>
+      <c r="A70" s="44"/>
+      <c r="B70" s="45"/>
       <c r="C70" s="12"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="33"/>
-      <c r="F70" s="33"/>
-      <c r="G70" s="33"/>
-      <c r="H70" s="33"/>
-      <c r="I70" s="33"/>
-      <c r="J70" s="34"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="38"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="38"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="38"/>
+      <c r="J70" s="38"/>
     </row>
     <row r="71" spans="1:10" ht="15" thickBot="1">
-      <c r="A71" s="48"/>
-      <c r="B71" s="49"/>
+      <c r="A71" s="39"/>
+      <c r="B71" s="40"/>
       <c r="C71" s="13"/>
-      <c r="D71" s="27"/>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="27"/>
-      <c r="H71" s="27"/>
-      <c r="I71" s="27"/>
-      <c r="J71" s="28"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
+      <c r="I71" s="38"/>
+      <c r="J71" s="38"/>
     </row>
     <row r="73" spans="1:10" ht="15">
       <c r="A73" s="2" t="s">
@@ -2034,11 +2022,11 @@
       </c>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="62"/>
-      <c r="B74" s="62"/>
-      <c r="E74" s="62"/>
-      <c r="F74" s="62"/>
-      <c r="G74" s="62"/>
+      <c r="A74" s="41"/>
+      <c r="B74" s="41"/>
+      <c r="E74" s="41"/>
+      <c r="F74" s="41"/>
+      <c r="G74" s="41"/>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="1" t="s">
@@ -2049,55 +2037,45 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="89">
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A55:J55"/>
-    <mergeCell ref="D59:G59"/>
-    <mergeCell ref="H57:J57"/>
-    <mergeCell ref="H58:J58"/>
-    <mergeCell ref="H59:J59"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="H56:J56"/>
+  <mergeCells count="101">
+    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="H69:J69"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="H70:J70"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="H71:J71"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="H66:J66"/>
+    <mergeCell ref="D67:G67"/>
+    <mergeCell ref="H67:J67"/>
+    <mergeCell ref="D68:G68"/>
+    <mergeCell ref="H68:J68"/>
+    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="D64:G64"/>
+    <mergeCell ref="H64:J64"/>
+    <mergeCell ref="D65:G65"/>
+    <mergeCell ref="H65:J65"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A38:J38"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="D60:G60"/>
+    <mergeCell ref="H60:J60"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="H61:J61"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="H62:J62"/>
     <mergeCell ref="D57:G57"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="E9:F9"/>
@@ -2113,34 +2091,56 @@
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D64:J64"/>
-    <mergeCell ref="A38:J38"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="D71:J71"/>
-    <mergeCell ref="A8:J8"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="D65:J65"/>
-    <mergeCell ref="D66:J66"/>
-    <mergeCell ref="D67:J67"/>
-    <mergeCell ref="D68:J68"/>
-    <mergeCell ref="D69:J69"/>
-    <mergeCell ref="D70:J70"/>
-    <mergeCell ref="D60:J60"/>
-    <mergeCell ref="D61:J61"/>
-    <mergeCell ref="D62:J62"/>
-    <mergeCell ref="D63:J63"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A55:J55"/>
+    <mergeCell ref="D59:G59"/>
+    <mergeCell ref="H57:J57"/>
+    <mergeCell ref="H58:J58"/>
+    <mergeCell ref="H59:J59"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="H56:J56"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I34:J34"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Número de caracteres" error="Excedió los 150 caracteres permitidos." sqref="B14:J14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>150</formula1>
     </dataValidation>
@@ -2153,6 +2153,9 @@
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Número de caracteres" error="Excedió los 300 caracteres permitiods." sqref="B20:J20" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>300</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9 D40:G53 D31:G36" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.19685039370078741" bottom="0.31496062992125984" header="0.19685039370078741" footer="0.19685039370078741"/>
@@ -2161,41 +2164,5 @@
     <oddFooter>Página &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E40:E53 E31:E36</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>F40:F53 F31:F36</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000009000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>G40:G53 G31:G36</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D40:D53 D31:D36</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>